<commit_message>
readme change and DR 1 change
</commit_message>
<xml_diff>
--- a/Test_Documentation/Defect_Reports/DefectReports_like_web_for_STA_course.xlsx
+++ b/Test_Documentation/Defect_Reports/DefectReports_like_web_for_STA_course.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lilia\Documents\I-Tester_Portfolio\Portfolio_Tester\Test_Documentation\Defect_Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01505203-CF8C-47E7-AD8E-56F9A9DFFF3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C395254-2D80-4B74-835C-06394F395CBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37770" yWindow="-3800" windowWidth="37770" windowHeight="20360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19290" yWindow="-4320" windowWidth="19380" windowHeight="20970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bugs. Testing courses" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="130">
   <si>
     <t>ID</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Symptom</t>
   </si>
   <si>
-    <t xml:space="preserve">Summary </t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -79,9 +76,6 @@
   </si>
   <si>
     <t>1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X  </t>
   </si>
   <si>
     <t>Functional
@@ -110,10 +104,6 @@
 The button for checkout is absent, and the user can't continue ordering.
 Reproducibility: Always.
 Workaround: No.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The cart should have a visible button to proceed to the checkout or place an order.
-The button should be clearly visible, prominently placed, and labeled with clear and concise text such as "Proceed to Checkout" or "Place Your Order", etc. </t>
   </si>
   <si>
     <t>In the cart there are no any buttons available to proceed to checkout or place an order.</t>
@@ -272,14 +262,6 @@
     <t>Incorrect currency is displayed for the item "Men's Vintage Ethnic Print Zip Pocket Plush Lined Thermal Jacket" in the cart.</t>
   </si>
   <si>
-    <t>The currency used on the site during this test is the USD.
-The item "Men's Vintage Ethnic Print Zip Pocket Plush Lined Thermal Jacket" in the cart has the price "€ 53.89" in EUR. Presumably this is a discounted price, but the discount label "Free Gift" is missing.
-Also, this item has a second price "$67.89" in dollars in gray color, which is crossed out. Presumably this is a  price without discount.
-The final price for the item (black color) is also "€ 53.89" in EUR.
- displayed in EUR, despite the currency chosen on the site is USD. 
-Other prices in the shopping list are displayed in USD correctly.</t>
-  </si>
-  <si>
     <t>STR:
 1. Set the currency for site prices to USD or check that it's already set.
 2. Find the item "Men's Vintage Ethnic Print Zip Pocket Plush Lined Thermal Jacket" in the shopping list (Catalog).
@@ -300,12 +282,6 @@
     <t>Major</t>
   </si>
   <si>
-    <t xml:space="preserve">2 ways to explain the defect are possible:
-1. Incorrect conversion in EUR.
-2. Incorrect mark  "€", but correct price.
-</t>
-  </si>
-  <si>
     <t>6</t>
   </si>
   <si>
@@ -313,9 +289,6 @@
   </si>
   <si>
     <t>Unfriendly behavior</t>
-  </si>
-  <si>
-    <t>A "Free Gift" label is missing for the item  in the cart that has a discount.</t>
   </si>
   <si>
     <t>The calculation section of the cart have a position: Free Gift "-$11.89".
@@ -330,14 +303,6 @@
 The discount amount is also not specified.</t>
   </si>
   <si>
-    <t>STR:
-1. Find the item "Men's Vintage Ethnic Print Zip Pocket Plush Lined Thermal Jacket" in the shopping list or catalog.
-2. See the price of this item.
-Defect:  the item has two prices, but there is no information about discount with the "Free Gift" label. 
-Reproducibility: Always.
-Workaround: No.</t>
-  </si>
-  <si>
     <t>The prices with a discount should have the "Free Gift" label with a tag image.</t>
   </si>
   <si>
@@ -358,44 +323,6 @@
 5 units of goods in the cart: 1 + 1 +2 + 1 .
 There are four individual items of goods in the cart, except for item "I Would Like To Apologize To Anyone I Have Not Yet Offended Men's Short Sleeve T-Shirt", which has a quantity of two.
 Such a mismatch can cause confusion for the user.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve">STR:
-1. Add 4 items of goods to the cart (quantity: 1 + 1 + 2 + 1) according to the screenshot.
-2. Check the cart icon with the counter on the top right of the page.
-Defect: the number of items in the cart and the number of  the counter on the cart icon are different.
-Reproducibility: Always.
-Workaround: Yes.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve">Note: 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>It's difficult to say without more context and interactions with the functionality, but some possible actions that could reproduce the bug are:
-- adding items to the cart and then removing the;
-- adding items to the cart and then changing the quantity of one or more items;
-- adding items to the cart from different pages on the site;
-- navigating away from the cart page and then returning to it.</t>
-    </r>
   </si>
   <si>
     <t>The counter on the cart icon should display the right amount of units of goods from the cart as "5".</t>
@@ -419,19 +346,6 @@
     <t>The incorrect calculation result of "Subtotal" value in the calculation section of the cart.</t>
   </si>
   <si>
-    <t>The "Subtotal" value shows the overall price of the goods added to the cart without discounts ("Free gift").
-The subtotal price of all goods in the shopping list of the cart is displaying an amount lower than expected.
-There are four individual items of goods in the cart, except for item № 3 "I Would Like To Apologize To Anyone I Have Not Yet Offended Men's Short Sleeve T-Shirt", which has a quantity of two:
-1 + 1  + 2 + 1 = 5 units
-Also item № 2 have a discount. 
-Items of  goods have the following prices (numbers according to the screenshot), which should be taken into account in the "Subtotal" value :
-item №1 - $72.89 
-item №2 - € 67.89 (because the "Free gift" discount is specified in a separate line in the calculation) 
-item №3 -  $51.78 (for two units) 
-item №4 - $20.89 
-Subtotal: = $213.45</t>
-  </si>
-  <si>
     <t>STR:
 1. Add 4 items of goods to the cart (quantity: 1 + 1 + 2 + 1) according to the screenshot.
 2. Add up all the prices taking into account the quantity of goods, but excluding discounts.
@@ -449,28 +363,11 @@
 Subtotal: $211.34</t>
   </si>
   <si>
-    <t xml:space="preserve">When calculating, it is necessary to take into account the currency.
-It could be the reason for the incorrect calculation: different price currencies and conversion from EUR to USD in the calculation.
-Since item № 2 is now reflected in EUR, the "Subtotal" value may change if this item's price is corrected in USD. </t>
-  </si>
-  <si>
     <t>9</t>
   </si>
   <si>
     <t xml:space="preserve">The incorrect amount of the "Free Gift" value in the calculation section. 
 </t>
-  </si>
-  <si>
-    <t>The item "Men's Vintage Ethnic Print Zip Pocket Plush Lined Thermal Jacket" in the shopping list of the cart has two prices. 
-The "€ 53.89" price has red color and "€" currency mark. 
-The "$67.89" price is crossed out and has a gray color, "$" currency mark.
-So, the "€ 53.89" price is the price with discount.
-The calculation section of the cart have a position: Free Gift "-$11.89".
-However, the difference between the price with a discount (€ 53.89) and the price without a discount ($67.89) for this item is 14. 
-It is only mathematical difference excluding  conversion to another currency.
-The discount amount is also not specified.
-It is unknown at what rate USD are converted into EUR and back.
-It is also not clear for sure whether a conversion was made between currencies or whether the currency mark is displayed incorrectly, and the conversion was not performed.</t>
   </si>
   <si>
     <t>STR: 
@@ -484,58 +381,200 @@
 Workaround: No.</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>1. In the case if currency mark is displayed incorrectly, and the conversion was not performed (67.89 - 53.89):
+    <t>"Free Gift" value in the calculation section is: $11.89</t>
+  </si>
+  <si>
+    <t>When calculating, it is necessary to take into account the currency.
+It could be the reason for the incorrect "Free Gift" value: different price currencies and conversion from EUR to USD in the calculation.</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The incorrect calculation result of "Total" value in the calculation section of the cart.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Total" value in the calculation section is correct: 
+$199.45 "Total"
+</t>
+  </si>
+  <si>
+    <t>"Total" value in the calculation section is incorrect: 
+$299.45</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>UI</t>
+  </si>
+  <si>
+    <t>Cosmetic flaw</t>
+  </si>
+  <si>
+    <t>The item "Men's Vintage Ethnic Print Zip Pocket Plush Lined Thermal Jacket" in the shopping list of the cart has the following description in the cart:
+ "Photo Color / L".
+Items in the shopping list in the cart have description tamplete that follows the format "Color / Size".
+However, the "Photo Color" label does not describe this item, but describes the photo.</t>
+  </si>
+  <si>
+    <t>An appropriate description of the item "Men's Vintage Ethnic Print Zip Pocket Plush Lined Thermal Jacket" in the shopping list of the cart:
+Ethnic Print / L</t>
+  </si>
+  <si>
+    <t>The description of the item "Men's Vintage Ethnic Print Zip Pocket Plush Lined Thermal Jacket" in the shopping list of the cart:
+Photo Color / L</t>
+  </si>
+  <si>
+    <t>Minor</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>To change description in the cart, it will be enough to change the indication of the color of the item on the name page of this one.</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>The color and size are not specified for the item "I Would Like To Apologize To Anyone I Have Not Yet Offended Men's Short Sleeve T-Shirt" when adding it to the cart.</t>
+  </si>
+  <si>
+    <t>Items in the shopping list in the cart have description template that follows the format "Color / Size".
+However, the item "I Would Like To Apologize To Anyone I Have Not Yet Offended Men's Short Sleeve T-Shirt" does not have such description as "Color / Size".</t>
+  </si>
+  <si>
+    <t>STR: 
+1. Find the item "I Would Like To Apologize To Anyone I Have Not Yet Offended Men's Short Sleeve T-Shirt" in the catalog.
+2. Add this item to the cart.
+3. Check what description this item has in the shopping list of the cart.
+Defect: The color and size information is absent for this item.
+Reproducibility: Always.
+Workaround: No.</t>
+  </si>
+  <si>
+    <t>The description of the item "I Would Like To Apologize To Anyone I Have Not Yet Offended Men's Short Sleeve T-Shirt" is absent in the shopping list of the cart.</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>Missing links or clickable elements in the item names within the cart do not allow users to open the corresponding product page.</t>
+  </si>
+  <si>
+    <t>When the user adds an item to the cart and then clicks on the cart icon to view the cart contents, the name of the item is displayed but there is no link or clickable element associated with the name to open the corresponding product page. 
+This means that users cannot view additional information about the product, such as product details or reviews, from the cart page.</t>
+  </si>
+  <si>
+    <t>STR:
+1. Add any items from catalog to the cart.
+2. View the shopping cart page.
+3. Click on any item name in the cart.
+Defect: No link or clickable element in the item name.
+Reproducibility: Always.
+Workaround: No.</t>
+  </si>
+  <si>
+    <t>Clicking on the item name from the cart should open the corresponding item page.</t>
+  </si>
+  <si>
+    <t>Clicking on the item name from the cart does not follow to the corresponding item page.</t>
+  </si>
+  <si>
+    <t>Back on main page</t>
+  </si>
+  <si>
+    <t>Practical task on the testing courses: Create complete bug reports for the bugs you find in the screenshots below. That is, bugs were searched using a screenshot.</t>
+  </si>
+  <si>
+    <t>Summary</t>
+  </si>
+  <si>
+    <t>The cart should have a visible button to proceed to the checkout or place an order.
+The button should be clearly visible, prominently placed, and labeled with clear and concise text such as "Proceed to Checkout" or "Place Your Order", etc.</t>
+  </si>
+  <si>
+    <t>The currency used on the site during this test is the USD.
+The item "Men's Vintage Ethnic Print Zip Pocket Plush Lined Thermal Jacket" in the cart has the price "€ 53.89" in EUR. Presumably this is a discounted price, but the discount label "Free Gift" is missing.
+Also, this item has a second price "$67.89" in dollars in gray color, which is crossed out. Presumably this is a price without discount.
+The final price for the item (black color) is also "€ 53.89" in EUR.
+ displayed in EUR, despite the currency chosen on the site is USD. 
+Other prices in the shopping list are displayed in USD correctly.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 ways to explain the defect are possible:
+1. Incorrect conversion in EUR.
+2. Incorrect mark "€", but correct price.
+</t>
+  </si>
+  <si>
+    <t>A "Free Gift" label is missing for the item in the cart that has a discount.</t>
+  </si>
+  <si>
+    <t>STR:
+1. Find the item "Men's Vintage Ethnic Print Zip Pocket Plush Lined Thermal Jacket" in the shopping list or catalog.
+2. See the price of this item.
+Defect: the item has two prices, but there is no information about discount with the "Free Gift" label. 
+Reproducibility: Always.
+Workaround: No.</t>
+  </si>
+  <si>
+    <t>STR:
+1. Add 4 items of goods to the cart (quantity: 1 + 1 + 2 + 1) according to the screenshot.
+2. Check the cart icon with the counter on the top right of the page.
+Defect: the number of items in the cart and the number of the counter on the cart icon are different.
+Reproducibility: Always.
+Workaround: Yes.
+Note: 
+It's difficult to say without more context and interactions with the functionality, but some possible actions that could reproduce the bug are:
+- adding items to the cart and then removing the;
+- adding items to the cart and then changing the quantity of one or more items;
+- adding items to the cart from different pages on the site;
+- navigating away from the cart page and then returning to it.</t>
+  </si>
+  <si>
+    <t>The "Subtotal" value shows the overall price of the goods added to the cart without discounts ("Free gift").
+The subtotal price of all goods in the shopping list of the cart is displaying an amount lower than expected.
+There are four individual items of goods in the cart, except for item № 3 "I Would Like To Apologize To Anyone I Have Not Yet Offended Men's Short Sleeve T-Shirt", which has a quantity of two:
+1 + 1 + 2 + 1 = 5 units
+Also item № 2 have a discount. 
+Items of goods have the following prices (numbers according to the screenshot), which should be taken into account in the "Subtotal" value :
+item №1 - $72.89 
+item №2 - € 67.89 (because the "Free gift" discount is specified in a separate line in the calculation) 
+item №3 - $51.78 (for two units) 
+item №4 - $20.89 
+Subtotal: = $213.45</t>
+  </si>
+  <si>
+    <t>The item "Men's Vintage Ethnic Print Zip Pocket Plush Lined Thermal Jacket" in the shopping list of the cart has two prices. 
+The "€ 53.89" price has red color and "€" currency mark. 
+The "$67.89" price is crossed out and has a gray color, "$" currency mark.
+So, the "€ 53.89" price is the price with discount.
+The calculation section of the cart have a position: Free Gift "-$11.89".
+However, the difference between the price with a discount (€ 53.89) and the price without a discount ($67.89) for this item is 14. 
+It is only mathematical difference excluding conversion to another currency.
+The discount amount is also not specified.
+It is unknown at what rate USD are converted into EUR and back.
+It is also not clear for sure whether a conversion was made between currencies or whether the currency mark is displayed incorrectly, and the conversion was not performed.</t>
+  </si>
+  <si>
+    <t>1. In the case if currency mark is displayed incorrectly, and the conversion was not performed (67.89 - 53.89):
 Free Gift: 14 (mathematical difference excluding currency).
-2. In case the  conversion was made between currencies:
+2. In case the conversion was made between currencies:
 Now the rate is not known.
-Let use mid-market rate on April, 06, 2023</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>from Google Currency Converter (https://www.google.com/search?q=currency+converter) 
+Let use mid-market rate on April, 06, 2023 from Google Currency Converter (https://www.google.com/search?q=currency+converter) 
 53.89 Euros =
 58.76 US Dollars
 (1 EUR = 1.09 USD)
 So, $67.89 - $58.79 = $9.13</t>
-    </r>
-  </si>
-  <si>
-    <t>"Free Gift" value in the calculation section is: $11.89</t>
-  </si>
-  <si>
-    <t>When calculating, it is necessary to take into account the currency.
-It could be the reason for the incorrect "Free Gift" value: different price currencies and conversion from EUR to USD in the calculation.</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The incorrect calculation result of "Total" value in the calculation section of the cart.
-</t>
   </si>
   <si>
     <t xml:space="preserve">A "Total" value in the calculation section of the cart shows the total price of the items added to the shopping cart minus discounts. 
 Whereas the subtotal shows the total price of the products without discounts.
 And it is also common in online stores to include in the total shipping cost and/or taxes.
-In the calculation section there is no mentions of  total shipping cost and/or taxes.
+In the calculation section there is no mentions of total shipping cost and/or taxes.
 The total in this calculation section is calculated as follows:
 "Subtotal" value minus "Free Sift" value = "Total" value.
 After adding goods to the cart according to the screenshot, the "Total" value is calculated incorrectly.
@@ -547,7 +586,7 @@
   <si>
     <t>STR:
 1. Add 4 items of goods to the cart (quantity: 1 + 1 + 2 + 1) according to the screenshot.
-2. Deduct the "Free Gift" value  from the "Subtotal" value from the calculation subsection of the cart.
+2. Deduct the "Free Gift" value from the "Subtotal" value from the calculation subsection of the cart.
 3. Compere the result of this deduction with the "Total" value.
 4. Sum up all the final prices for each item of the goods (the last numbers for each item are in black).
 5. Compere the result of this summing with the "Total" value.
@@ -556,42 +595,11 @@
 Workaround: No.</t>
   </si>
   <si>
-    <t xml:space="preserve">"Total" value in the calculation section is correct: 
-$199.45 "Total"
-</t>
-  </si>
-  <si>
-    <t>"Total" value in the calculation section is incorrect: 
-$299.45</t>
-  </si>
-  <si>
-    <t>The "Total" amount may contain hidden payments that are not shown to the user like shipping cost and/or taxes.
-Even if this values are zero, it is better to reflect them to make the price more clear to buyers. 
-The unexpected hidden cost is one of the major reasons why customers abandon the checkout process. According to the Baymard’s research (https://baymard.com/lists/cart-abandonment-rate), extra hidden costs such as shipping charge, tax, transaction fee hold the highest percentage (55%) amongst the reasons for abandonment during checkout.
-Still, most of the eCommerce stores do not reveal the actual order total up-front before the payment page in the checkout process. The best place to reveal the estimated cost of the cart is right after a customer selects the shipping option. 
-If you cannot provide an estimate, add a shipping calculator tool that customers can use to find out their total purchase cost.</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>UI</t>
-  </si>
-  <si>
-    <t>Cosmetic flaw</t>
-  </si>
-  <si>
-    <t>The color of the item "Men's Vintage Ethnic Print Zip Pocket Plush Lined Thermal Jacket" is specified incorrectly  when adding it to the cart.</t>
-  </si>
-  <si>
-    <t>The item "Men's Vintage Ethnic Print Zip Pocket Plush Lined Thermal Jacket" in the shopping list of the cart has the following description in the cart:
- "Photo Color / L".
-Items in the shopping list in the cart have description tamplete that follows the format "Color / Size".
-However, the "Photo Color" label does not describe this item, but describes the photo.</t>
+    <t>The color of the item "Men's Vintage Ethnic Print Zip Pocket Plush Lined Thermal Jacket" is specified incorrectly when adding it to the cart.</t>
   </si>
   <si>
     <t>STR:
-1. Find the item "Men's Vintage Ethnic Print Zip Pocket Plush Lined Thermal Jacket"  in the catalog.
+1. Find the item "Men's Vintage Ethnic Print Zip Pocket Plush Lined Thermal Jacket" in the catalog.
 2. Add this item to the cart.
 3. Check the color description of this item.
 Defect: Incorrect color specification. 
@@ -599,95 +607,37 @@
 Workaround: No.</t>
   </si>
   <si>
-    <t>An appropriate description of the item "Men's Vintage Ethnic Print Zip Pocket Plush Lined Thermal Jacket" in the shopping list of the cart:
-Ethnic Print / L</t>
-  </si>
-  <si>
-    <t>The description of the item "Men's Vintage Ethnic Print Zip Pocket Plush Lined Thermal Jacket" in the shopping list of the cart:
-Photo Color / L</t>
-  </si>
-  <si>
-    <t>Minor</t>
-  </si>
-  <si>
-    <t>Low</t>
-  </si>
-  <si>
-    <t>To change description in the cart, it will be enough to change the indication of the color of the item on the name page of this one.</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>The color and size are not specified for the item "I Would Like To Apologize To Anyone I Have Not Yet Offended Men's Short Sleeve T-Shirt" when adding it to the cart.</t>
-  </si>
-  <si>
-    <t>Items in the shopping list in the cart have description template that follows the format "Color / Size".
-However, the item "I Would Like To Apologize To Anyone I Have Not Yet Offended Men's Short Sleeve T-Shirt" does not have such description as "Color / Size".</t>
-  </si>
-  <si>
-    <t>STR: 
-1. Find the item "I Would Like To Apologize To Anyone I Have Not Yet Offended Men's Short Sleeve T-Shirt" in the catalog.
-2. Add this item to the cart.
-3. Check what description this item has in the shopping list of the cart.
-Defect: The color and size information is absent for this item.
-Reproducibility: Always.
-Workaround: No.</t>
-  </si>
-  <si>
-    <t>A description of the item  "I Would Like To Apologize To Anyone I Have Not Yet Offended Men's Short Sleeve T-Shirt" in the shopping list of the cart is:
+    <t>A description of the item "I Would Like To Apologize To Anyone I Have Not Yet Offended Men's Short Sleeve T-Shirt" in the shopping list of the cart is:
 "Black / S"
 OR
 "Black with white lettering / S"</t>
   </si>
   <si>
-    <t>The description of the item "I Would Like To Apologize To Anyone I Have Not Yet Offended Men's Short Sleeve T-Shirt" is absent in the shopping list of the cart.</t>
-  </si>
-  <si>
     <t>Check the page of this item.
-Perhaps there is no mention of the color and size directly in the product description and  the T-shirt is presented only in one color and size.
+Perhaps there is no mention of the color and size directly in the product description and the T-shirt is presented only in one color and size.
 P.s. In the real work, the tester would check it themself.</t>
   </si>
   <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>Missing links or clickable elements in the item names within the cart do not allow users to open the corresponding product page.</t>
-  </si>
-  <si>
-    <t>When the user adds an item to the cart and then clicks on the cart icon to view the cart contents, the name of the item is displayed but there is no link or clickable element associated with the name to open the corresponding product page. 
-This means that users cannot view additional information about the product, such as product details or reviews, from the cart page.</t>
-  </si>
-  <si>
-    <t>STR:
-1. Add any items from catalog to the cart.
-2. View the shopping cart page.
-3. Click on any item name in the cart.
-Defect: No link or clickable element in the item name.
-Reproducibility: Always.
-Workaround: No.</t>
-  </si>
-  <si>
-    <t>Clicking on the item name from the cart should open the corresponding item page.</t>
-  </si>
-  <si>
-    <t>Clicking on the item name from the cart does not follow to the corresponding item page.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This defect has an impact on the user experience as it prevents users from easily accessing additional information about products from the cart page. </t>
-  </si>
-  <si>
-    <t>Back on main page</t>
-  </si>
-  <si>
-    <t>Practical task on the testing courses: Create complete bug reports for the bugs you find in the screenshots below. That is, bugs were searched using a screenshot.</t>
+    <t>This defect has an impact on the user experience as it prevents users from easily accessing additional information about products from the cart page.</t>
+  </si>
+  <si>
+    <t>The "Total" amount may contain hidden payments that are not shown to the user like shipping cost and/or taxes.
+Even if this values are zero, it is better to reflect them to make the price more clear to buyers. 
+The unexpected hidden cost is one of the major reasons why customers abandon the checkout process. According to the Baymard's research (https://baymard.com/lists/cart-abandonment-rate), extra hidden costs such as shipping charge, tax, transaction fee hold the highest percentage (55%) amongst the reasons for abandonment during checkout.
+Still, most of the eCommerce stores do not reveal the actual order total up-front before the payment page in the checkout process. The best place to reveal the estimated cost of the cart is right after a customer selects the shipping option. 
+If you cannot provide an estimate, add a shipping calculator tool that customers can use to find out their total purchase cost.</t>
+  </si>
+  <si>
+    <t>When calculating, it is necessary to take into account the currency.
+It could be the reason for the incorrect calculation: different price currencies and conversion from EUR to USD in the calculation.
+Since item № 2 is now reflected in EUR, the "Subtotal" value may change if this item's price is corrected in USD.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -742,12 +692,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -841,7 +785,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -911,22 +855,22 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1936,7 +1880,7 @@
   <sheetData>
     <row r="1" spans="1:15" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="28" t="s">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="B1" s="28"/>
       <c r="C1" s="28"/>
@@ -1951,7 +1895,7 @@
       <c r="L1" s="28"/>
       <c r="M1" s="28"/>
       <c r="N1" s="27" t="s">
-        <v>129</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
@@ -1971,617 +1915,617 @@
         <v>4</v>
       </c>
       <c r="F2" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="G2" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="H2" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="I2" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="18" t="s">
+      <c r="J2" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="18" t="s">
+      <c r="K2" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="18" t="s">
+      <c r="L2" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="18" t="s">
+      <c r="M2" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="19" t="s">
+      <c r="N2" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="19" t="s">
+      <c r="O2" s="18" t="s">
         <v>13</v>
-      </c>
-      <c r="O2" s="18" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="362.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="E3" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="F3" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="G3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="23" t="s">
+      <c r="H3" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="I3" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="J3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="24" t="s">
+      <c r="K3" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="L3" s="8" t="s">
         <v>23</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="L3" s="8" t="s">
-        <v>26</v>
       </c>
       <c r="M3" s="15"/>
       <c r="N3" s="15"/>
       <c r="O3" s="13" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="362.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="F4" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F4" s="23" t="s">
+      <c r="I4" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="J4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K4" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="L4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M4" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="K4" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>37</v>
       </c>
       <c r="N4" s="15"/>
       <c r="O4" s="13" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="333.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="3" t="s">
+      <c r="F5" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="G5" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="H5" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="F5" s="23" t="s">
+      <c r="I5" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="J5" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="K5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="M5" s="5" t="s">
         <v>44</v>
-      </c>
-      <c r="I5" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="J5" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="M5" s="5" t="s">
-        <v>47</v>
       </c>
       <c r="N5" s="17"/>
       <c r="O5" s="13" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="409.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" s="8" t="s">
+      <c r="H6" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="F6" s="23" t="s">
+      <c r="I6" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="J6" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="K6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="M6" s="5" t="s">
         <v>52</v>
-      </c>
-      <c r="I6" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="J6" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="M6" s="5" t="s">
-        <v>55</v>
       </c>
       <c r="N6" s="6"/>
       <c r="O6" s="13" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="372" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="3" t="s">
+      <c r="F7" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="G7" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="H7" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="I7" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="F7" s="23" t="s">
+      <c r="J7" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="K7" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="H7" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="K7" s="11" t="s">
-        <v>65</v>
-      </c>
       <c r="L7" s="11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="M7" s="9" t="s">
-        <v>66</v>
+        <v>114</v>
       </c>
       <c r="N7" s="3"/>
       <c r="O7" s="13" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="399" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F8" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="H8" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="J8" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="16" t="s">
+      <c r="K8" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="L8" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="M8" s="9" t="s">
         <v>68</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="F8" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="H8" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="K8" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="L8" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="M8" s="9" t="s">
-        <v>75</v>
       </c>
       <c r="N8" s="3"/>
       <c r="O8" s="13" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="22" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F9" s="23" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="H9" s="14" t="s">
-        <v>79</v>
+        <v>117</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="K9" s="11" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="L9" s="11" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="M9" s="11" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="N9" s="3"/>
       <c r="O9" s="13" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="393" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="22" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F10" s="23" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>85</v>
+        <v>118</v>
       </c>
       <c r="H10" s="14" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="K10" s="11" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="L10" s="11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="M10" s="20" t="s">
-        <v>89</v>
+        <v>129</v>
       </c>
       <c r="N10" s="17"/>
       <c r="O10" s="13" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="399.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F11" s="23" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>92</v>
+        <v>119</v>
       </c>
       <c r="H11" s="14" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>94</v>
+        <v>120</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="K11" s="11" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="L11" s="11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="M11" s="20" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="N11" s="3"/>
       <c r="O11" s="13" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="409.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="22" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F12" s="23" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="G12" s="25" t="s">
-        <v>99</v>
+        <v>121</v>
       </c>
       <c r="H12" s="26" t="s">
-        <v>100</v>
+        <v>122</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="K12" s="11" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="L12" s="11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="M12" s="20" t="s">
-        <v>103</v>
+        <v>128</v>
       </c>
       <c r="N12" s="3"/>
       <c r="O12" s="13" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="369" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="22" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="F13" s="23" t="s">
-        <v>107</v>
+        <v>123</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="H13" s="14" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="K13" s="11" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
       <c r="L13" s="11" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
       <c r="M13" s="20" t="s">
-        <v>114</v>
+        <v>97</v>
       </c>
       <c r="N13" s="3"/>
       <c r="O13" s="13" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="379.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="22" t="s">
-        <v>115</v>
+        <v>98</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="F14" s="23" t="s">
-        <v>116</v>
+        <v>99</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="H14" s="14" t="s">
-        <v>118</v>
+        <v>101</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>120</v>
+        <v>102</v>
       </c>
       <c r="K14" s="11" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
       <c r="L14" s="11" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
       <c r="M14" s="21" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="N14" s="3"/>
       <c r="O14" s="13" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="385.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="22" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F15" s="23" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="H15" s="14" t="s">
-        <v>125</v>
+        <v>106</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
       <c r="J15" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="K15" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="L15" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="M15" s="21" t="s">
         <v>127</v>
-      </c>
-      <c r="K15" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="L15" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="M15" s="21" t="s">
-        <v>128</v>
       </c>
       <c r="N15" s="3"/>
       <c r="O15" s="13" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>